<commit_message>
Modified UI file and moved functions
</commit_message>
<xml_diff>
--- a/bin/essential data/4-Leg Template.xlsx
+++ b/bin/essential data/4-Leg Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\External Shiz\Programming\Traffic TVC\bin\essential data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7C38A9-716D-4857-B14B-3CC5D373A85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B64F0F-EB94-4330-9BC1-D98890D86905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +573,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>8</v>

</xml_diff>